<commit_message>
switch all labels and buttons to pics
</commit_message>
<xml_diff>
--- a/Patients.xlsx
+++ b/Patients.xlsx
@@ -9,7 +9,7 @@
     <sheet name="patient_details_and_exercises" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -440,10 +440,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
@@ -466,85 +466,90 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>gender</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>number of exercises</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>bend_elbows_ball</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>raise_arms_above_head_ball</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>raise_arms_forward_turn_ball</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>open_arms_and_forward_ball</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>open_arms_above_head_ball</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>open_arms_with_band</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>open_arms_and_up_with_band</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>up_with_band_and_lean</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>bend_elbows_stick</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>bend_elbows_and_up_stick</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>arms_up_and_down_stick</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>switch_with_stick</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>hands_behind_and_lean_notool</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>right_hand_up_and_bend_notool</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>left_hand_up_and_bend_notool</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>raising_hands_diagonally_notool</t>
         </is>
@@ -564,10 +569,12 @@
           <t>כהן</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="b">
@@ -583,10 +590,10 @@
         <v>1</v>
       </c>
       <c r="J2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" t="b">
         <v>0</v>
@@ -598,7 +605,7 @@
         <v>0</v>
       </c>
       <c r="O2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" t="b">
         <v>0</v>
@@ -613,14 +620,15 @@
         <v>0</v>
       </c>
       <c r="T2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>11223344</t>
-        </is>
+      <c r="A3" t="n">
+        <v>11223344</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -632,14 +640,16 @@
           <t>כהן</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
       </c>
       <c r="F3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -681,6 +691,9 @@
         <v>0</v>
       </c>
       <c r="T3" t="b">
+        <v>0</v>
+      </c>
+      <c r="U3" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>